<commit_message>
added alm and tp
added alm and tp
</commit_message>
<xml_diff>
--- a/Table_calculations.xlsx
+++ b/Table_calculations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjgru\Documents\5thYear\CODESIGN\FinalProject\Codesign_FinalProj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjgru\Documents\5thYear\CODESIGN\Codesign_FinalProj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D77E5C4A-5307-43EA-85B7-E06910926A58}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C586026-4B94-4323-9646-CA754EC292DE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21580" windowHeight="9800" xr2:uid="{7FA98631-8571-415C-A9F1-D612E764E0AF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>50MHz</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Throughput (Mb/s)</t>
+  </si>
+  <si>
+    <t>TP/A</t>
+  </si>
+  <si>
+    <t>ALM</t>
   </si>
 </sst>
 </file>
@@ -419,19 +425,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56FD37CF-80E1-42CA-84B5-7EED78C76C48}">
-  <dimension ref="C3:G9"/>
+  <dimension ref="C3:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
         <v>1</v>
       </c>
@@ -439,7 +447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
         <v>0</v>
       </c>
@@ -448,7 +456,7 @@
         <v>2E-8</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
         <v>3</v>
       </c>
@@ -461,8 +469,14 @@
       <c r="G6" t="s">
         <v>9</v>
       </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>4</v>
       </c>
@@ -481,13 +495,43 @@
         <f>F7/1000000</f>
         <v>4.6495408578402876E-2</v>
       </c>
+      <c r="H7">
+        <v>691</v>
+      </c>
+      <c r="I7">
+        <f>G7/H7</f>
+        <v>6.7287132530250183E-5</v>
+      </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>5</v>
       </c>
+      <c r="D8">
+        <f>188+35215</f>
+        <v>35403</v>
+      </c>
+      <c r="E8">
+        <f>D8*E4</f>
+        <v>7.0806000000000005E-4</v>
+      </c>
+      <c r="F8">
+        <f>128/E8</f>
+        <v>180775.64048244499</v>
+      </c>
+      <c r="G8">
+        <f>F8/1000000</f>
+        <v>0.18077564048244499</v>
+      </c>
+      <c r="H8">
+        <v>1821</v>
+      </c>
+      <c r="I8">
+        <f>G8/H8</f>
+        <v>9.9272729534566161E-5</v>
+      </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>6</v>
       </c>
@@ -505,6 +549,13 @@
       <c r="G9">
         <f>F9/1000000</f>
         <v>4.6947323635776798E-2</v>
+      </c>
+      <c r="H9">
+        <v>805</v>
+      </c>
+      <c r="I9">
+        <f>G9/H9</f>
+        <v>5.831965669040596E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>